<commit_message>
Correção das datas para primeira coluna nas data table
</commit_message>
<xml_diff>
--- a/primeiraRevisao.xlsx
+++ b/primeiraRevisao.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D692FE3-AD88-4716-83CC-2F77AECC745E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A9B1E4-3B84-47DE-BC7B-D526D58B323E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="29">
   <si>
     <t>Colocar CNPJ na busca</t>
   </si>
@@ -98,16 +98,52 @@
   </si>
   <si>
     <t>Adicionar Limite de crédito, observação, Tipo de Envio: [ Carro Metalmax, Transportadora, Sedex, Retirar  ]</t>
+  </si>
+  <si>
+    <t>ver local</t>
+  </si>
+  <si>
+    <t>ver cadastro</t>
+  </si>
+  <si>
+    <t>Bloquear campo Nome contato e Responsável Metalmax</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -133,9 +169,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -418,10 +473,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="A12" sqref="A12:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -456,7 +511,7 @@
       <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -470,7 +525,7 @@
       <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" s="6" t="s">
         <v>4</v>
       </c>
     </row>
@@ -484,6 +539,9 @@
       <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="D4" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -495,16 +553,22 @@
       <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="1" t="s">
+      <c r="D5" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="4" t="s">
         <v>9</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
@@ -514,8 +578,11 @@
       <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="7" t="s">
         <v>10</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
@@ -526,7 +593,10 @@
         <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
@@ -534,10 +604,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
@@ -548,7 +621,10 @@
         <v>15</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
@@ -559,7 +635,10 @@
         <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
@@ -567,10 +646,10 @@
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
@@ -581,7 +660,10 @@
         <v>17</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
@@ -592,7 +674,10 @@
         <v>17</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
@@ -603,7 +688,7 @@
         <v>17</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
@@ -614,10 +699,22 @@
         <v>17</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
commit conserto dos problemas listados
</commit_message>
<xml_diff>
--- a/primeiraRevisao.xlsx
+++ b/primeiraRevisao.xlsx
@@ -1,26 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A9B1E4-3B84-47DE-BC7B-D526D58B323E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51EFF036-DD55-45EF-96C4-912EF5367392}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="31">
   <si>
     <t>Colocar CNPJ na busca</t>
   </si>
@@ -100,13 +105,19 @@
     <t>Adicionar Limite de crédito, observação, Tipo de Envio: [ Carro Metalmax, Transportadora, Sedex, Retirar  ]</t>
   </si>
   <si>
-    <t>ver local</t>
-  </si>
-  <si>
-    <t>ver cadastro</t>
-  </si>
-  <si>
     <t>Bloquear campo Nome contato e Responsável Metalmax</t>
+  </si>
+  <si>
+    <t>Acertar a tela principal</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>Principal</t>
+  </si>
+  <si>
+    <t>verificar folha</t>
   </si>
 </sst>
 </file>
@@ -149,12 +160,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -169,7 +186,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -191,6 +208,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -473,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:D12"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -487,7 +510,7 @@
     <col min="4" max="4" width="11.7265625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -501,7 +524,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -515,7 +538,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -529,7 +552,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -539,11 +562,11 @@
       <c r="C4" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D4" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -553,11 +576,11 @@
       <c r="C5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="D5" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -571,7 +594,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -585,7 +608,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -593,13 +616,13 @@
         <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -613,7 +636,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -627,7 +650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -641,7 +664,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -651,8 +674,14 @@
       <c r="C12" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -666,7 +695,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -680,18 +709,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>17</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="D15" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -701,8 +733,11 @@
       <c r="C16" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="D16" s="6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>8</v>
       </c>
@@ -711,6 +746,23 @@
       </c>
       <c r="C17" s="1" t="s">
         <v>21</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>